<commit_message>
order maken half getest
</commit_message>
<xml_diff>
--- a/Opdracht/Eigen documentatie/Planning.xlsx
+++ b/Opdracht/Eigen documentatie/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lasa\Desktop\Turing_Machine\Java\dorb\Opdracht\Eigen documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F5CB57-6D7B-404D-8E7D-118A8AC9E11B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C67616-6202-48B3-928A-99D6184F4DA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Testen</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Crud: rit (date)(id)</t>
+  </si>
+  <si>
+    <t>Optimaliseer login</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="180"/>
@@ -321,6 +324,7 @@
       <alignment textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -635,11 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1551,8 +1555,8 @@
       <c r="AM21" s="6"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>16</v>
+      <c r="A22" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>2</v>
@@ -1597,9 +1601,9 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="6"/>
@@ -1614,9 +1618,9 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -1636,13 +1640,13 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="6"/>
       <c r="AM23" s="6"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>2</v>
@@ -1660,12 +1664,12 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="U24" s="16"/>
+      <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
@@ -1681,12 +1685,15 @@
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
       <c r="AJ24" s="6"/>
+      <c r="AK24" s="6"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="6"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="6"/>
@@ -1704,11 +1711,11 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
+      <c r="R25" s="16"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
+      <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
@@ -1722,10 +1729,11 @@
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>2</v>
@@ -1748,7 +1756,7 @@
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
+      <c r="U26" s="16"/>
       <c r="V26" s="16"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -1766,7 +1774,7 @@
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>2</v>
@@ -1790,8 +1798,8 @@
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="6"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
@@ -1802,11 +1810,12 @@
       <c r="AE27" s="6"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="6"/>
-      <c r="AI27" s="11"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
-        <v>7</v>
+      <c r="A28" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>2</v>
@@ -1846,7 +1855,7 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>2</v>
@@ -1871,8 +1880,8 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="6"/>
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
       <c r="AA29" s="6"/>
@@ -1885,10 +1894,10 @@
       <c r="AI29" s="11"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
@@ -1917,38 +1926,50 @@
       <c r="Z30" s="6"/>
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AI30" s="11"/>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
+      <c r="A31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="16"/>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1971,10 +1992,38 @@
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
       <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AB32" s="9"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+    </row>
+    <row r="33" spans="3:28" x14ac:dyDescent="0.3">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="9"/>
+      <c r="Y33" s="9"/>
+      <c r="Z33" s="9"/>
+      <c r="AA33" s="9"/>
+      <c r="AB33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>